<commit_message>
Update parts for availability
Signed-off-by: Tisham Dhar <whatnickd@gmail.com>
</commit_message>
<xml_diff>
--- a/ATM90E36_Breakout/bom/ATM90E36_Breakout.xlsx
+++ b/ATM90E36_Breakout/bom/ATM90E36_Breakout.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
   <si>
     <t xml:space="preserve">Sourced</t>
   </si>
@@ -88,6 +88,15 @@
     <t xml:space="preserve">R0603</t>
   </si>
   <si>
+    <t xml:space="preserve">R26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0201JR-0710KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10K</t>
+  </si>
+  <si>
     <t xml:space="preserve">R10, R12, R14</t>
   </si>
   <si>
@@ -106,15 +115,6 @@
     <t xml:space="preserve">1K</t>
   </si>
   <si>
-    <t xml:space="preserve">R26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SR0603KR-7W10KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10K</t>
-  </si>
-  <si>
     <t xml:space="preserve">R36</t>
   </si>
   <si>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">Q1</t>
   </si>
   <si>
-    <t xml:space="preserve">FA-128 16.00M-A0NNNNHB0REB</t>
+    <t xml:space="preserve">ECS-160-10-36-CKM-TR</t>
   </si>
   <si>
     <t xml:space="preserve">FA-128</t>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t xml:space="preserve">CTA1, CTB1, CTC1, CTN1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-PJ-342</t>
   </si>
   <si>
     <t xml:space="preserve">ST-PJ-312</t>
@@ -277,13 +280,13 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="30.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -406,7 +409,7 @@
         <v>21</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -426,7 +429,7 @@
         <v>21</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -446,7 +449,7 @@
         <v>21</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,7 +463,7 @@
         <v>32</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>33</v>
@@ -480,7 +483,7 @@
         <v>35</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>33</v>
@@ -577,10 +580,10 @@
         <v>51</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>4</v>

</xml_diff>